<commit_message>
Updates to concept maps this the new extension elements
Updates to concept maps this the new extension elements
</commit_message>
<xml_diff>
--- a/src-models/idea4rc-models-and-maps.xlsx
+++ b/src-models/idea4rc-models-and-maps.xlsx
@@ -5,13 +5,12 @@
   <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Roberta\HL7EU\IDEA4RC\idea4rc2025\idea4rc\src-models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Roberta\HL7EU\ScriptPython\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF14DADD-26D1-4E2E-9296-2BBBE4B2D1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5A4ECD-A152-4E40-A1E1-64BA38D7EB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="25" activeTab="25" xr2:uid="{DBDA221E-EFE5-4A34-8B86-7FDF16AB25A8}"/>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="32" activeTab="35" xr2:uid="{5AC1C6E0-0B35-4ABC-AFF0-9D917C4380C0}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="33" activeTab="37" xr2:uid="{DBDA221E-EFE5-4A34-8B86-7FDF16AB25A8}"/>
   </bookViews>
   <sheets>
     <sheet name="ConceptMaps" sheetId="15" r:id="rId1"/>
@@ -4511,9 +4510,6 @@
     <t>It must be calculated from the update of the same MedicationAdministration</t>
   </si>
   <si>
-    <t>AdverseEvent.extension:OccurrenceR5</t>
-  </si>
-  <si>
     <t>Condition.onset</t>
   </si>
   <si>
@@ -4691,9 +4687,6 @@
     <t>Observation.extension:sameHospital</t>
   </si>
   <si>
-    <t>MedicationAdministration.dosage.extension:timing.repeat.count</t>
-  </si>
-  <si>
     <t xml:space="preserve">Applicable only if Code is in ValueSet: Drugs for Treatments </t>
   </si>
   <si>
@@ -4706,22 +4699,28 @@
     <t>See group for Observation: Number of tumor nodules</t>
   </si>
   <si>
-    <t>Procedure.extension:adaptive</t>
-  </si>
-  <si>
-    <t>If it is present an observation with value = 36769249 'Transit Metastasis with Clinical Confirmation', it is ''true'', else 'false'</t>
+    <t>AdverseEvent.extension:occurrence</t>
+  </si>
+  <si>
+    <t>Procedure.extension:adaptive.value</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/adverseEvent-eu-i4rc</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/locoRegional-category</t>
+  </si>
+  <si>
+    <t>isolatedLimbPerfusion2FHIR</t>
   </si>
   <si>
     <t>If it is present a procedure with code 4263386 'Sentinel lymph node biopsy' related to the observation, it is 'true'</t>
   </si>
   <si>
-    <t>isolatedLimbPerfusion2FHIR</t>
-  </si>
-  <si>
-    <t>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/adverseEvent-eu-i4rc</t>
-  </si>
-  <si>
-    <t>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/locoRegional-category</t>
+    <t>If it is present an observation with value = 32943 'Invasive Disease', it is ''true'', else 'false'</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.dosage.extension:chemotherapyTiming.value.repeat.count</t>
   </si>
 </sst>
 </file>
@@ -4809,18 +4808,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -4948,7 +4941,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5003,24 +4996,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5054,7 +5046,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5070,9 +5062,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5499,11 +5488,8 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
-    <sheetView topLeftCell="A5" workbookViewId="1">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5520,31 +5506,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="37" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5552,10 +5538,10 @@
       <c r="A2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="39" t="str">
+      <c r="C2" s="38" t="str">
         <f t="shared" ref="C2:C19" si="0">"http://hl7.eu/fhir/ig/idea4rc/ConceptMap/"&amp;A2</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/ConceptMap/subject2FHIR</v>
       </c>
@@ -5568,11 +5554,11 @@
       <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="39" t="str">
+      <c r="G2" s="38" t="str">
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!A2</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/Subject</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="38" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -5583,10 +5569,10 @@
       <c r="A3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="39" t="str">
+      <c r="C3" s="38" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.eu/fhir/ig/idea4rc/ConceptMap/followup2FHIR</v>
       </c>
@@ -5599,11 +5585,11 @@
       <c r="F3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="39" t="str">
+      <c r="G3" s="38" t="str">
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!A3</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PatientFollowUp</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="38" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="8" t="s">
@@ -5614,10 +5600,10 @@
       <c r="A4" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="39" t="str">
+      <c r="C4" s="38" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.eu/fhir/ig/idea4rc/ConceptMap/hospitalPatientRecords2FHIR</v>
       </c>
@@ -5630,26 +5616,26 @@
       <c r="F4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="39" t="str">
+      <c r="G4" s="38" t="str">
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!A4</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/HospitalPatientRecords</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="38" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="40"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="39" t="str">
+      <c r="C5" s="38" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.eu/fhir/ig/idea4rc/ConceptMap/diagnosis2FHIR</v>
       </c>
@@ -5662,11 +5648,11 @@
       <c r="F5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="39" t="str">
+      <c r="G5" s="38" t="str">
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!A6</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/Diagnosis</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="38" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="8" t="s">
@@ -5677,30 +5663,30 @@
       <c r="A6" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="41" t="str">
+      <c r="C6" s="40" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.eu/fhir/ig/idea4rc/ConceptMap/cancerEpisode2FHIR</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="42" t="s">
+      <c r="F6" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="41" t="str">
+      <c r="G6" s="40" t="str">
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!A5</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/CancerEpisode</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="41" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5860,10 +5846,10 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="52" t="s">
         <v>916</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="43" t="s">
         <v>917</v>
       </c>
       <c r="C12" s="13" t="str">
@@ -5876,7 +5862,7 @@
       <c r="E12" s="3" t="s">
         <v>919</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="44" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="13" t="str">
@@ -5891,10 +5877,10 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="52" t="s">
         <v>921</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="43" t="s">
         <v>922</v>
       </c>
       <c r="C13" s="13" t="str">
@@ -5907,7 +5893,7 @@
       <c r="E13" s="3" t="s">
         <v>924</v>
       </c>
-      <c r="F13" s="45" t="s">
+      <c r="F13" s="44" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="13" t="str">
@@ -5922,10 +5908,10 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="52" t="s">
         <v>925</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="43" t="s">
         <v>926</v>
       </c>
       <c r="C14" s="13" t="str">
@@ -5938,7 +5924,7 @@
       <c r="E14" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="F14" s="44" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="13" t="str">
@@ -5956,7 +5942,7 @@
       <c r="A15" s="34" t="s">
         <v>930</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="43" t="s">
         <v>931</v>
       </c>
       <c r="C15" s="13" t="str">
@@ -5969,7 +5955,7 @@
       <c r="E15" s="3" t="s">
         <v>933</v>
       </c>
-      <c r="F15" s="45" t="s">
+      <c r="F15" s="44" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="13" t="str">
@@ -5984,10 +5970,10 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="52" t="s">
         <v>939</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="43" t="s">
         <v>934</v>
       </c>
       <c r="C16" s="13" t="str">
@@ -6000,7 +5986,7 @@
       <c r="E16" s="3" t="s">
         <v>935</v>
       </c>
-      <c r="F16" s="45" t="s">
+      <c r="F16" s="44" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="13" t="str">
@@ -6018,7 +6004,7 @@
       <c r="A17" s="34" t="s">
         <v>940</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="43" t="s">
         <v>938</v>
       </c>
       <c r="C17" s="13" t="str">
@@ -6031,7 +6017,7 @@
       <c r="E17" s="3" t="s">
         <v>942</v>
       </c>
-      <c r="F17" s="45" t="s">
+      <c r="F17" s="44" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="13" t="str">
@@ -6046,10 +6032,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="52" t="s">
         <v>943</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="43" t="s">
         <v>944</v>
       </c>
       <c r="C18" s="13" t="str">
@@ -6062,7 +6048,7 @@
       <c r="E18" s="3" t="s">
         <v>946</v>
       </c>
-      <c r="F18" s="45" t="s">
+      <c r="F18" s="44" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="13" t="str">
@@ -6077,10 +6063,10 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
-        <v>1214</v>
-      </c>
-      <c r="B19" s="44" t="s">
+      <c r="A19" s="52" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B19" s="43" t="s">
         <v>947</v>
       </c>
       <c r="C19" s="13" t="str">
@@ -6093,7 +6079,7 @@
       <c r="E19" s="3" t="s">
         <v>949</v>
       </c>
-      <c r="F19" s="45" t="s">
+      <c r="F19" s="44" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="13" t="str">
@@ -6196,7 +6182,6 @@
     <sheetView topLeftCell="B18" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7021,7 +7006,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7511,10 +7495,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B9"/>
-    </sheetView>
-    <sheetView topLeftCell="C1" workbookViewId="1">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7655,13 +7636,13 @@
         <v>118</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="B6" s="17" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="C6" s="2" t="str">
         <f>DiseaseExtentI4RC!A4</f>
@@ -7685,10 +7666,10 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/DiseaseExtent</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>1216</v>
-      </c>
-      <c r="C7" s="64" t="str">
+      <c r="B7" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C7" s="62" t="str">
         <f>DiseaseExtentI4RC!A5</f>
         <v>locoRegional</v>
       </c>
@@ -7700,11 +7681,11 @@
         <v>1087</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>1200</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -7712,8 +7693,8 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/DiseaseExtent</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>1216</v>
+      <c r="B8" s="2" t="s">
+        <v>1212</v>
       </c>
       <c r="C8" s="2" t="str">
         <f>DiseaseExtentI4RC!A6</f>
@@ -7727,11 +7708,11 @@
         <v>1087</v>
       </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>1212</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -7739,8 +7720,8 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/DiseaseExtent</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>1216</v>
+      <c r="B9" s="2" t="s">
+        <v>1212</v>
       </c>
       <c r="C9" s="2" t="str">
         <f>DiseaseExtentI4RC!A7</f>
@@ -7754,11 +7735,11 @@
         <v>1087</v>
       </c>
       <c r="F9" s="14"/>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -8052,7 +8033,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8206,9 +8186,6 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-    <sheetView topLeftCell="C1" workbookViewId="1">
-      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8348,7 +8325,7 @@
         <v>114</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -8400,7 +8377,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8866,9 +8842,6 @@
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A6" sqref="A1:XFD1048576"/>
-    </sheetView>
-    <sheetView topLeftCell="C12" workbookViewId="1">
-      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8976,14 +8949,14 @@
         <v>Gene expression analysis performed (R)</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
         <v>118</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -9002,15 +8975,15 @@
         <f>GeneticTestExpressionI4RC!D5</f>
         <v>Date of Gene expression (O)</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="41" t="s">
         <v>1024</v>
       </c>
-      <c r="F5" s="42"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>114</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -9030,14 +9003,14 @@
         <v>Gene mutation analysis performed (R)</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="8" t="s">
         <v>118</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -9064,7 +9037,7 @@
         <v>114</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -9084,14 +9057,14 @@
         <v>Tests for chromosome translocations performed (R)</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="8" t="s">
         <v>118</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -9118,7 +9091,7 @@
         <v>114</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -9138,14 +9111,14 @@
         <v>Next generation sequencing (NGS)  performed (R)</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="8" t="s">
         <v>118</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -9172,7 +9145,7 @@
         <v>114</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -9192,14 +9165,14 @@
         <v>Polymerase chain reaction (PCR) test performed (R)</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="8" t="s">
         <v>118</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -9226,7 +9199,7 @@
         <v>114</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -9246,14 +9219,14 @@
         <v>Immunohistochemistry  performed (R)</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="8" t="s">
         <v>118</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -9280,7 +9253,7 @@
         <v>114</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -9300,14 +9273,14 @@
         <v>Circulating Tumour DNA (ctDNA) performed (R)</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="8" t="s">
         <v>118</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -9334,7 +9307,7 @@
         <v>114</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
   </sheetData>
@@ -9358,7 +9331,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9514,7 +9486,6 @@
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9638,7 +9609,7 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/EpisodeEvent</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>112</v>
       </c>
       <c r="C5" s="33" t="s">
@@ -9649,7 +9620,7 @@
         <v>Defined At (O)</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14" t="s">
@@ -9675,7 +9646,7 @@
         <v>Date of episode (M)</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14" t="s">
@@ -9795,148 +9766,147 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59" style="49" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="49" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="49" customWidth="1"/>
-    <col min="5" max="5" width="59.7109375" style="50" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="49" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="49"/>
-    <col min="8" max="8" width="15.85546875" style="49" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="49"/>
+    <col min="1" max="1" width="59" style="48" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="48" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="48" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="48" customWidth="1"/>
+    <col min="5" max="5" width="59.7109375" style="49" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="48" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="48"/>
+    <col min="8" max="8" width="15.85546875" style="48" customWidth="1"/>
+    <col min="9" max="16384" width="8.7109375" style="48"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="51" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="49" t="s">
         <v>950</v>
       </c>
-      <c r="F2" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="49" t="s">
+      <c r="F2" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>394</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>99</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="48" t="s">
         <v>395</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="49" t="s">
         <v>1014</v>
       </c>
-      <c r="F3" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="49" t="s">
+      <c r="F3" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="48" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="48" t="s">
         <v>396</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="48" t="s">
         <v>397</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="49" t="s">
         <v>1016</v>
       </c>
-      <c r="F4" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="49" t="s">
+      <c r="F4" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="48" t="s">
         <v>398</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="48" t="s">
         <v>399</v>
       </c>
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="49" t="s">
         <v>1015</v>
       </c>
-      <c r="F5" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="49" t="s">
+      <c r="F5" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="48" t="s">
         <v>393</v>
       </c>
     </row>
@@ -9953,9 +9923,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
-    <sheetView topLeftCell="A9" workbookViewId="1">
-      <selection activeCell="A14" sqref="A1:D19"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9966,16 +9933,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>4</v>
       </c>
     </row>
@@ -10290,7 +10257,6 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0"/>
-    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10452,7 +10418,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10655,10 +10620,9 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4:E5"/>
     </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10986,7 +10950,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11140,7 +11103,6 @@
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11187,7 +11149,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/OverallTreatmentResponse</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C2" s="14" t="str">
         <f>OverallTreatmentResponseI4RC!A2</f>
@@ -11212,7 +11174,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/OverallTreatmentResponse</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C3" s="14" t="str">
         <f>OverallTreatmentResponseI4RC!A3</f>
@@ -11237,13 +11199,13 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/OverallTreatmentResponse</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>1204</v>
-      </c>
-      <c r="C4" s="58" t="str">
+        <v>1203</v>
+      </c>
+      <c r="C4" s="57" t="str">
         <f>OverallTreatmentResponseI4RC!A4</f>
         <v>overallTreatmentResponse</v>
       </c>
-      <c r="D4" s="59" t="str">
+      <c r="D4" s="58" t="str">
         <f>OverallTreatmentResponseI4RC!D4</f>
         <v>Overall Treatment response (based on imaging alone; no recist or other criteria) (M)</v>
       </c>
@@ -11254,7 +11216,7 @@
       <c r="G4" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="H4" s="58"/>
+      <c r="H4" s="57"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="str">
@@ -11262,7 +11224,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/OverallTreatmentResponse</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C5" s="14" t="str">
         <f>OverallTreatmentResponseI4RC!A5</f>
@@ -11289,7 +11251,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/OverallTreatmentResponse</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C6" s="14" t="str">
         <f>OverallTreatmentResponseI4RC!A5</f>
@@ -11300,7 +11262,7 @@
         <v>Overall Treatment response defined/done (M)</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14" t="s">
@@ -11415,7 +11377,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12111,11 +12072,8 @@
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
-    <sheetView topLeftCell="B12" workbookViewId="1">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12445,7 +12403,7 @@
         <v>118</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -12526,7 +12484,7 @@
         <v>118</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -12553,7 +12511,7 @@
         <v>118</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -12562,7 +12520,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PathologicalStage</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="C17" s="14" t="str">
         <f>PathologicalStageI4RC!A11</f>
@@ -12587,7 +12545,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PathologicalStage</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="C18" s="14" t="str">
         <f>PathologicalStageI4RC!A12</f>
@@ -12601,11 +12559,11 @@
         <v>1087</v>
       </c>
       <c r="F18" s="14"/>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -12614,7 +12572,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PathologicalStage</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="C19" s="14" t="str">
         <f>PathologicalStageI4RC!A13</f>
@@ -12628,11 +12586,11 @@
         <v>1087</v>
       </c>
       <c r="F19" s="14"/>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -12641,7 +12599,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PathologicalStage</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="C20" s="14" t="str">
         <f>PathologicalStageI4RC!A14</f>
@@ -12655,11 +12613,11 @@
         <v>1087</v>
       </c>
       <c r="F20" s="14"/>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -13004,252 +12962,251 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59" style="49" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="49" customWidth="1"/>
-    <col min="4" max="4" width="66" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.7109375" style="50" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="49" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="49"/>
-    <col min="8" max="8" width="15.42578125" style="49" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="49"/>
+    <col min="1" max="1" width="59" style="48" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="48" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="48" customWidth="1"/>
+    <col min="4" max="4" width="66" style="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.7109375" style="49" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="48" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="48"/>
+    <col min="8" max="8" width="15.42578125" style="48" customWidth="1"/>
+    <col min="9" max="16384" width="8.7109375" style="48"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="47" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="54" t="s">
         <v>362</v>
       </c>
-      <c r="F2" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="54" t="s">
+      <c r="F2" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="53" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="53" t="s">
         <v>363</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="53" t="s">
         <v>364</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="54" t="s">
         <v>365</v>
       </c>
-      <c r="F3" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="54" t="s">
+      <c r="F3" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="53" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="53" t="s">
         <v>367</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="53" t="s">
         <v>99</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="53" t="s">
         <v>368</v>
       </c>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="54" t="s">
         <v>369</v>
       </c>
-      <c r="F4" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="54" t="s">
+      <c r="F4" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="53" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="53" t="s">
         <v>371</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="53" t="s">
         <v>372</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="54" t="s">
         <v>373</v>
       </c>
-      <c r="F5" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="54" t="s">
+      <c r="F5" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="53" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="53" t="s">
         <v>374</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="53" t="s">
         <v>175</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="53" t="s">
         <v>375</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="54" t="s">
         <v>376</v>
       </c>
-      <c r="F6" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="54" t="s">
+      <c r="F6" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="53" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="53" t="s">
         <v>379</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="54" t="s">
         <v>380</v>
       </c>
-      <c r="F7" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="54" t="s">
+      <c r="F7" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="H7" s="54" t="s">
+      <c r="H7" s="53" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="53" t="s">
         <v>381</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="53" t="s">
         <v>382</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="54" t="s">
         <v>383</v>
       </c>
-      <c r="F8" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="54" t="s">
+      <c r="F8" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="53" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="54" t="s">
         <v>385</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="53" t="s">
         <v>99</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="53" t="s">
         <v>386</v>
       </c>
-      <c r="E9" s="55" t="s">
+      <c r="E9" s="54" t="s">
         <v>387</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="G9" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="54" t="s">
+      <c r="G9" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="53" t="s">
         <v>101</v>
       </c>
     </row>
@@ -13257,7 +13214,7 @@
       <c r="C11" s="3"/>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C24" s="54"/>
+      <c r="C24" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13271,10 +13228,9 @@
   </sheetPr>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13319,7 +13275,7 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PatientFollowUp</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="55" t="s">
         <v>349</v>
       </c>
       <c r="C2" s="2" t="str">
@@ -13344,7 +13300,7 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PatientFollowUp</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="55" t="s">
         <v>349</v>
       </c>
       <c r="C3" s="2" t="str">
@@ -13362,7 +13318,7 @@
       <c r="G3" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="H3" s="57" t="s">
+      <c r="H3" s="56" t="s">
         <v>1132</v>
       </c>
     </row>
@@ -13371,7 +13327,7 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PatientFollowUp</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="55" t="s">
         <v>349</v>
       </c>
       <c r="C4" s="2" t="str">
@@ -13396,7 +13352,7 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PatientFollowUp</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="55" t="s">
         <v>349</v>
       </c>
       <c r="C5" s="2" t="str">
@@ -13414,7 +13370,7 @@
       <c r="G5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="H5" s="57" t="s">
+      <c r="H5" s="56" t="s">
         <v>1030</v>
       </c>
     </row>
@@ -13423,7 +13379,7 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PatientFollowUp</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="55" t="s">
         <v>349</v>
       </c>
       <c r="C6" s="2" t="str">
@@ -13450,7 +13406,7 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PatientFollowUp</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="55" t="s">
         <v>349</v>
       </c>
       <c r="C7" s="2" t="str">
@@ -13504,7 +13460,7 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PatientFollowUp</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="55" t="s">
         <v>112</v>
       </c>
       <c r="C9" s="5" t="str">
@@ -13531,7 +13487,7 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PatientFollowUp</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="55" t="s">
         <v>112</v>
       </c>
       <c r="C10" s="5" t="str">
@@ -13558,7 +13514,7 @@
         <f>"http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/PatientFollowUp</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="55" t="s">
         <v>112</v>
       </c>
       <c r="C11" s="5" t="str">
@@ -13770,7 +13726,6 @@
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A4" sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14628,7 +14583,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14666,13 +14620,13 @@
     </row>
     <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B2" t="s">
         <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="D2" t="s">
         <v>868</v>
@@ -14782,9 +14736,6 @@
   <sheetViews>
     <sheetView topLeftCell="B10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-    <sheetView topLeftCell="B11" workbookViewId="1">
-      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14842,7 +14793,7 @@
         <f>RadiotherapyI4RC!D2</f>
         <v>Diagnosis reference (M)</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="63" t="s">
         <v>407</v>
       </c>
       <c r="F2" s="14"/>
@@ -14867,7 +14818,7 @@
         <f>RadiotherapyI4RC!D3</f>
         <v>Episode Event reference (M)</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="64" t="s">
         <v>407</v>
       </c>
       <c r="F3" s="3"/>
@@ -15153,7 +15104,7 @@
         <v>Adaptive RT (O)</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="24" t="s">
@@ -15685,7 +15636,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15890,7 +15840,6 @@
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16215,1313 +16164,1310 @@
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A17" sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView topLeftCell="B13" workbookViewId="1">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59" style="49" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="49" customWidth="1"/>
-    <col min="4" max="4" width="66" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.7109375" style="50" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="49" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="49"/>
-    <col min="8" max="8" width="80.7109375" style="49" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="49"/>
+    <col min="1" max="1" width="59" style="48" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="48" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="48" customWidth="1"/>
+    <col min="4" max="4" width="66" style="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.7109375" style="49" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="48" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="48"/>
+    <col min="8" max="8" width="80.7109375" style="48" customWidth="1"/>
+    <col min="9" max="16384" width="8.7109375" style="48"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="47" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="48" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="48" t="s">
         <v>232</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="48" t="s">
         <v>972</v>
       </c>
-      <c r="F2" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="49" t="s">
+      <c r="F2" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="48" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>234</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="48" t="s">
         <v>973</v>
       </c>
-      <c r="F3" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="49" t="s">
+      <c r="F3" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="48" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="48" t="s">
         <v>237</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="48" t="s">
         <v>239</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="48" t="s">
         <v>974</v>
       </c>
-      <c r="F4" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="49" t="s">
+      <c r="F4" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="48" t="s">
         <v>240</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="E5" s="48" t="s">
         <v>975</v>
       </c>
-      <c r="F5" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="49" t="s">
+      <c r="F5" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="48" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="48" t="s">
         <v>244</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="48" t="s">
         <v>976</v>
       </c>
-      <c r="F6" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="49" t="s">
+      <c r="F6" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="48" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="48" t="s">
         <v>246</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="48" t="s">
         <v>247</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="48" t="s">
         <v>977</v>
       </c>
-      <c r="F7" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="49" t="s">
+      <c r="F7" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="48" t="s">
         <v>248</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="48" t="s">
         <v>249</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="48" t="s">
         <v>978</v>
       </c>
-      <c r="F8" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="49" t="s">
+      <c r="F8" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="48" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="49" t="s">
         <v>251</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="48" t="s">
         <v>178</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="48" t="s">
         <v>252</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="48" t="s">
         <v>979</v>
       </c>
-      <c r="F9" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="49" t="s">
+      <c r="F9" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H9" s="49" t="s">
+      <c r="H9" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="48" t="s">
         <v>253</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="48" t="s">
         <v>254</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="48" t="s">
         <v>980</v>
       </c>
-      <c r="F10" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="49" t="s">
+      <c r="F10" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="48" t="s">
         <v>255</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="48" t="s">
         <v>99</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="48" t="s">
         <v>257</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="48" t="s">
         <v>981</v>
       </c>
-      <c r="F11" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="49" t="s">
+      <c r="F11" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H11" s="49" t="s">
+      <c r="H11" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="48" t="s">
         <v>258</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="48" t="s">
         <v>259</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="48" t="s">
         <v>982</v>
       </c>
-      <c r="F12" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="49" t="s">
+      <c r="F12" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H12" s="49" t="s">
+      <c r="H12" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="48" t="s">
         <v>260</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="48" t="s">
         <v>261</v>
       </c>
-      <c r="E13" s="49" t="str">
+      <c r="E13" s="48" t="str">
         <f t="array" ref="E13">"Previous cancer comorbidity related to "&amp;D13</f>
         <v>Previous cancer comorbidity related to Congestive heart failure (O)</v>
       </c>
-      <c r="F13" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="49" t="s">
+      <c r="F13" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H13" s="49" t="s">
+      <c r="H13" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="48" t="s">
         <v>262</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="48" t="s">
         <v>263</v>
       </c>
-      <c r="E14" s="49" t="str">
+      <c r="E14" s="48" t="str">
         <f t="array" ref="E14">"Previous cancer comorbidity related to "&amp;D14</f>
         <v>Previous cancer comorbidity related to Peripheral vascular disease (O)</v>
       </c>
-      <c r="F14" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="49" t="s">
+      <c r="F14" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H14" s="49" t="s">
+      <c r="H14" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="48" t="s">
         <v>264</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="48" t="s">
         <v>265</v>
       </c>
-      <c r="E15" s="49" t="str">
+      <c r="E15" s="48" t="str">
         <f t="array" ref="E15">"Previous cancer comorbidity related to "&amp;D15</f>
         <v>Previous cancer comorbidity related to Cerebrovascular accident  (except hemiplegia) (O)</v>
       </c>
-      <c r="F15" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="49" t="s">
+      <c r="F15" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H15" s="49" t="s">
+      <c r="H15" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="48" t="s">
         <v>266</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="48" t="s">
         <v>267</v>
       </c>
-      <c r="E16" s="49" t="str">
+      <c r="E16" s="48" t="str">
         <f t="array" ref="E16">"Previous cancer comorbidity related to "&amp;D16</f>
         <v>Previous cancer comorbidity related to Dementia (O)</v>
       </c>
-      <c r="F16" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="49" t="s">
+      <c r="F16" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="48" t="s">
         <v>268</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="48" t="s">
         <v>269</v>
       </c>
-      <c r="E17" s="49" t="str">
+      <c r="E17" s="48" t="str">
         <f t="array" ref="E17">"Previous cancer comorbidity related to "&amp;D17</f>
         <v>Previous cancer comorbidity related to Chronic pulmonary disease (O)</v>
       </c>
-      <c r="F17" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="49" t="s">
+      <c r="F17" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H17" s="49" t="s">
+      <c r="H17" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="48" t="s">
         <v>270</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="48" t="s">
         <v>271</v>
       </c>
-      <c r="E18" s="49" t="str">
+      <c r="E18" s="48" t="str">
         <f t="array" ref="E18">"Previous cancer comorbidity related to "&amp;D18</f>
         <v>Previous cancer comorbidity related to Connective tissue disease (O)</v>
       </c>
-      <c r="F18" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="49" t="s">
+      <c r="F18" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H18" s="49" t="s">
+      <c r="H18" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="48" t="s">
         <v>272</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="E19" s="49" t="str">
+      <c r="E19" s="48" t="str">
         <f t="array" ref="E19">"Previous cancer comorbidity related to "&amp;D19</f>
         <v>Previous cancer comorbidity related to Ulcer (O)</v>
       </c>
-      <c r="F19" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="49" t="s">
+      <c r="F19" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H19" s="49" t="s">
+      <c r="H19" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="48" t="s">
         <v>274</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="E20" s="49" t="str">
+      <c r="E20" s="48" t="str">
         <f t="array" ref="E20">"Previous cancer comorbidity related to "&amp;D20</f>
         <v>Previous cancer comorbidity related to Mild liver disease (O)</v>
       </c>
-      <c r="F20" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="49" t="s">
+      <c r="F20" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H20" s="49" t="s">
+      <c r="H20" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="48" t="s">
         <v>277</v>
       </c>
-      <c r="E21" s="49" t="str">
+      <c r="E21" s="48" t="str">
         <f t="array" ref="E21">"Previous cancer comorbidity related to "&amp;D21</f>
         <v>Previous cancer comorbidity related to Moderate to severe liver disease (O)</v>
       </c>
-      <c r="F21" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="49" t="s">
+      <c r="F21" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H21" s="49" t="s">
+      <c r="H21" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="48" t="s">
         <v>278</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="48" t="s">
         <v>279</v>
       </c>
-      <c r="E22" s="49" t="str">
+      <c r="E22" s="48" t="str">
         <f t="array" ref="E22">"Previous cancer comorbidity related to "&amp;D22</f>
         <v>Previous cancer comorbidity related to Diabetes (without complications) (O)</v>
       </c>
-      <c r="F22" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="49" t="s">
+      <c r="F22" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H22" s="49" t="s">
+      <c r="H22" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="48" t="s">
         <v>280</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="48" t="s">
         <v>281</v>
       </c>
-      <c r="E23" s="49" t="str">
+      <c r="E23" s="48" t="str">
         <f t="array" ref="E23">"Previous cancer comorbidity related to "&amp;D23</f>
         <v>Previous cancer comorbidity related to Diabetes with end organ damage (O)</v>
       </c>
-      <c r="F23" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="49" t="s">
+      <c r="F23" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H23" s="49" t="s">
+      <c r="H23" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="48" t="s">
         <v>282</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="E24" s="49" t="str">
+      <c r="E24" s="48" t="str">
         <f t="array" ref="E24">"Previous cancer comorbidity related to "&amp;D24</f>
         <v>Previous cancer comorbidity related to Hemiplegia (O)</v>
       </c>
-      <c r="F24" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="49" t="s">
+      <c r="F24" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H24" s="49" t="s">
+      <c r="H24" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="48" t="s">
         <v>284</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="48" t="s">
         <v>285</v>
       </c>
-      <c r="E25" s="49" t="str">
+      <c r="E25" s="48" t="str">
         <f t="array" ref="E25">"Previous cancer comorbidity related to "&amp;D25</f>
         <v>Previous cancer comorbidity related to Moderate to severe renal disease (O)</v>
       </c>
-      <c r="F25" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="49" t="s">
+      <c r="F25" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H25" s="49" t="s">
+      <c r="H25" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="48" t="s">
         <v>286</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D26" s="49" t="s">
+      <c r="D26" s="48" t="s">
         <v>287</v>
       </c>
-      <c r="E26" s="49" t="str">
+      <c r="E26" s="48" t="str">
         <f t="array" ref="E26">"Previous cancer comorbidity related to "&amp;D26</f>
         <v>Previous cancer comorbidity related to Solid tumor (non metastatic) (O)</v>
       </c>
-      <c r="F26" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="49" t="s">
+      <c r="F26" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H26" s="49" t="s">
+      <c r="H26" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="48" t="s">
         <v>288</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D27" s="49" t="s">
+      <c r="D27" s="48" t="s">
         <v>289</v>
       </c>
-      <c r="E27" s="49" t="str">
+      <c r="E27" s="48" t="str">
         <f t="array" ref="E27">"Previous cancer comorbidity related to "&amp;D27</f>
         <v>Previous cancer comorbidity related to Metastatic solid tumor (O)</v>
       </c>
-      <c r="F27" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="49" t="s">
+      <c r="F27" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H27" s="49" t="s">
+      <c r="H27" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="48" t="s">
         <v>290</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="E28" s="49" t="str">
+      <c r="E28" s="48" t="str">
         <f t="array" ref="E28">"Previous cancer comorbidity related to "&amp;D28</f>
         <v>Previous cancer comorbidity related to Leukemia (O)</v>
       </c>
-      <c r="F28" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="49" t="s">
+      <c r="F28" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H28" s="49" t="s">
+      <c r="H28" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D29" s="49" t="s">
+      <c r="D29" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E29" s="49" t="str">
+      <c r="E29" s="48" t="str">
         <f t="array" ref="E29">"Previous cancer comorbidity related to "&amp;D29</f>
         <v>Previous cancer comorbidity related to Lymphoma (O)</v>
       </c>
-      <c r="F29" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="49" t="s">
+      <c r="F29" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H29" s="49" t="s">
+      <c r="H29" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C30" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D30" s="49" t="s">
+      <c r="D30" s="48" t="s">
         <v>295</v>
       </c>
-      <c r="E30" s="49" t="str">
+      <c r="E30" s="48" t="str">
         <f t="array" ref="E30">"Previous cancer comorbidity related to "&amp;D30</f>
         <v>Previous cancer comorbidity related to Multiple myeloma (O)</v>
       </c>
-      <c r="F30" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="49" t="s">
+      <c r="F30" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H30" s="49" t="s">
+      <c r="H30" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="48" t="s">
         <v>296</v>
       </c>
-      <c r="B31" s="49" t="s">
+      <c r="B31" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C31" s="49" t="s">
+      <c r="C31" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D31" s="49" t="s">
+      <c r="D31" s="48" t="s">
         <v>297</v>
       </c>
-      <c r="E31" s="49" t="str">
+      <c r="E31" s="48" t="str">
         <f t="array" ref="E31">"Previous cancer comorbidity related to "&amp;D31</f>
         <v>Previous cancer comorbidity related to AIDS (O)</v>
       </c>
-      <c r="F31" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="49" t="s">
+      <c r="F31" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H31" s="49" t="s">
+      <c r="H31" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="48" t="s">
         <v>298</v>
       </c>
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="D32" s="49" t="s">
+      <c r="D32" s="48" t="s">
         <v>299</v>
       </c>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="48" t="s">
         <v>983</v>
       </c>
-      <c r="F32" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="49" t="s">
+      <c r="F32" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H32" s="49" t="s">
+      <c r="H32" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="48" t="s">
         <v>300</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D33" s="49" t="s">
+      <c r="D33" s="48" t="s">
         <v>301</v>
       </c>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="48" t="s">
         <v>983</v>
       </c>
-      <c r="F33" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="49" t="s">
+      <c r="F33" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H33" s="49" t="s">
+      <c r="H33" s="48" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="48" t="s">
         <v>303</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C34" s="49" t="s">
+      <c r="C34" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="D34" s="49" t="s">
+      <c r="D34" s="48" t="s">
         <v>304</v>
       </c>
-      <c r="E34" s="49" t="s">
+      <c r="E34" s="48" t="s">
         <v>984</v>
       </c>
-      <c r="F34" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="49" t="s">
+      <c r="F34" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H34" s="49" t="s">
+      <c r="H34" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="48" t="s">
         <v>305</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D35" s="49" t="s">
+      <c r="D35" s="48" t="s">
         <v>306</v>
       </c>
-      <c r="E35" s="49" t="s">
+      <c r="E35" s="48" t="s">
         <v>984</v>
       </c>
-      <c r="F35" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G35" s="49" t="s">
+      <c r="F35" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H35" s="49" t="s">
+      <c r="H35" s="48" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="48" t="s">
         <v>308</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D36" s="49" t="s">
+      <c r="D36" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="E36" s="49" t="s">
+      <c r="E36" s="48" t="s">
         <v>985</v>
       </c>
-      <c r="F36" s="49" t="s">
+      <c r="F36" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G36" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H36" s="49" t="s">
+      <c r="G36" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="48" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="48" t="s">
         <v>311</v>
       </c>
-      <c r="B37" s="49" t="s">
+      <c r="B37" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D37" s="49" t="s">
+      <c r="D37" s="48" t="s">
         <v>312</v>
       </c>
-      <c r="E37" s="49" t="s">
+      <c r="E37" s="48" t="s">
         <v>986</v>
       </c>
-      <c r="F37" s="49" t="s">
+      <c r="F37" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G37" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" s="49" t="s">
+      <c r="G37" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="48" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="48" t="s">
         <v>314</v>
       </c>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D38" s="49" t="s">
+      <c r="D38" s="48" t="s">
         <v>315</v>
       </c>
-      <c r="E38" s="49" t="s">
+      <c r="E38" s="48" t="s">
         <v>989</v>
       </c>
-      <c r="F38" s="49" t="s">
+      <c r="F38" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G38" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H38" s="49" t="s">
+      <c r="G38" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="48" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="48" t="s">
         <v>317</v>
       </c>
-      <c r="B39" s="49" t="s">
+      <c r="B39" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="49" t="s">
+      <c r="C39" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D39" s="49" t="s">
+      <c r="D39" s="48" t="s">
         <v>318</v>
       </c>
-      <c r="E39" s="49" t="s">
+      <c r="E39" s="48" t="s">
         <v>990</v>
       </c>
-      <c r="F39" s="49" t="s">
+      <c r="F39" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G39" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" s="49" t="s">
+      <c r="G39" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="48" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C40" s="49" t="s">
+      <c r="C40" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D40" s="49" t="s">
+      <c r="D40" s="48" t="s">
         <v>321</v>
       </c>
-      <c r="E40" s="49" t="s">
+      <c r="E40" s="48" t="s">
         <v>991</v>
       </c>
-      <c r="F40" s="49" t="s">
+      <c r="F40" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G40" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H40" s="49" t="s">
+      <c r="G40" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="48" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="48" t="s">
         <v>323</v>
       </c>
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D41" s="49" t="s">
+      <c r="D41" s="48" t="s">
         <v>324</v>
       </c>
-      <c r="E41" s="49" t="s">
+      <c r="E41" s="48" t="s">
         <v>992</v>
       </c>
-      <c r="F41" s="49" t="s">
+      <c r="F41" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G41" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H41" s="49" t="s">
+      <c r="G41" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="48" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="49" t="s">
+      <c r="A42" s="48" t="s">
         <v>326</v>
       </c>
-      <c r="B42" s="49" t="s">
+      <c r="B42" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D42" s="49" t="s">
+      <c r="D42" s="48" t="s">
         <v>327</v>
       </c>
-      <c r="E42" s="49" t="s">
+      <c r="E42" s="48" t="s">
         <v>993</v>
       </c>
-      <c r="F42" s="49" t="s">
+      <c r="F42" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G42" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H42" s="49" t="s">
+      <c r="G42" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="48" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="48" t="s">
         <v>329</v>
       </c>
-      <c r="B43" s="49" t="s">
+      <c r="B43" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C43" s="49" t="s">
+      <c r="C43" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D43" s="49" t="s">
+      <c r="D43" s="48" t="s">
         <v>330</v>
       </c>
-      <c r="E43" s="49" t="s">
+      <c r="E43" s="48" t="s">
         <v>994</v>
       </c>
-      <c r="F43" s="49" t="s">
+      <c r="F43" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G43" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H43" s="49" t="s">
+      <c r="G43" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="48" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="49" t="s">
+      <c r="A44" s="48" t="s">
         <v>332</v>
       </c>
-      <c r="B44" s="49" t="s">
+      <c r="B44" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C44" s="49" t="s">
+      <c r="C44" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D44" s="49" t="s">
+      <c r="D44" s="48" t="s">
         <v>333</v>
       </c>
-      <c r="E44" s="49" t="s">
+      <c r="E44" s="48" t="s">
         <v>995</v>
       </c>
-      <c r="F44" s="49" t="s">
+      <c r="F44" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G44" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H44" s="49" t="s">
+      <c r="G44" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="48" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="B45" s="49" t="s">
+      <c r="B45" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="49" t="s">
+      <c r="C45" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D45" s="49" t="s">
+      <c r="D45" s="48" t="s">
         <v>336</v>
       </c>
-      <c r="E45" s="49" t="s">
+      <c r="E45" s="48" t="s">
         <v>996</v>
       </c>
-      <c r="F45" s="49" t="s">
+      <c r="F45" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G45" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H45" s="49" t="s">
+      <c r="G45" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="48" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="49" t="s">
+      <c r="A46" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C46" s="49" t="s">
+      <c r="C46" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D46" s="49" t="s">
+      <c r="D46" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="E46" s="49" t="s">
+      <c r="E46" s="48" t="s">
         <v>997</v>
       </c>
-      <c r="F46" s="49" t="s">
+      <c r="F46" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G46" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H46" s="49" t="s">
+      <c r="G46" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="48" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="48" t="s">
         <v>341</v>
       </c>
-      <c r="B47" s="49" t="s">
+      <c r="B47" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C47" s="49" t="s">
+      <c r="C47" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D47" s="49" t="s">
+      <c r="D47" s="48" t="s">
         <v>342</v>
       </c>
-      <c r="E47" s="49" t="s">
+      <c r="E47" s="48" t="s">
         <v>998</v>
       </c>
-      <c r="F47" s="49" t="s">
+      <c r="F47" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G47" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H47" s="49" t="s">
+      <c r="G47" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="48" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="49" t="s">
+      <c r="A48" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="B48" s="49" t="s">
+      <c r="B48" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C48" s="49" t="s">
+      <c r="C48" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D48" s="49" t="s">
+      <c r="D48" s="48" t="s">
         <v>345</v>
       </c>
-      <c r="E48" s="49" t="s">
+      <c r="E48" s="48" t="s">
         <v>987</v>
       </c>
-      <c r="F48" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G48" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H48" s="49" t="s">
+      <c r="F48" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G48" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="48" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="49" t="s">
+      <c r="A49" s="48" t="s">
         <v>347</v>
       </c>
-      <c r="B49" s="49" t="s">
+      <c r="B49" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C49" s="49" t="s">
+      <c r="C49" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D49" s="49" t="s">
+      <c r="D49" s="48" t="s">
         <v>891</v>
       </c>
-      <c r="E49" s="49" t="s">
+      <c r="E49" s="48" t="s">
         <v>988</v>
       </c>
-      <c r="F49" s="49" t="s">
+      <c r="F49" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G49" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="H49" s="49" t="s">
+      <c r="G49" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="48" t="s">
         <v>348</v>
       </c>
     </row>
@@ -17538,10 +17484,9 @@
   </sheetPr>
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView topLeftCell="B36" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="A50" sqref="A50:XFD51"/>
     </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18851,7 +18796,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19676,11 +19620,8 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="B20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C11" sqref="C11:C15"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="1">
-      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19786,7 +19727,7 @@
         <v>Surgery type (M)</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14" t="s">
@@ -19956,14 +19897,14 @@
         <v>Tumor rupture (M)</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -20063,7 +20004,7 @@
         <v>118</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -20089,7 +20030,7 @@
         <v>118</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -20115,7 +20056,7 @@
         <v>118</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -20141,7 +20082,7 @@
         <v>114</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -20167,7 +20108,7 @@
         <v>118</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -20193,7 +20134,7 @@
         <v>118</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -20242,7 +20183,7 @@
         <v>118</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -20268,7 +20209,7 @@
         <v>118</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -20294,7 +20235,7 @@
         <v>118</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -20320,7 +20261,7 @@
         <v>118</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -20346,7 +20287,7 @@
         <v>118</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -20372,7 +20313,7 @@
         <v>118</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -20398,7 +20339,7 @@
         <v>118</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -20424,7 +20365,7 @@
         <v>118</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -20450,7 +20391,7 @@
         <v>118</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -20476,7 +20417,7 @@
         <v>118</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -20547,7 +20488,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20980,15 +20920,12 @@
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{410D113B-68AE-4993-B10D-204275957080}">
   <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21100,7 +21037,7 @@
         <v>1142</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H4" s="14"/>
@@ -21125,7 +21062,7 @@
         <v>1143</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H5" s="14"/>
@@ -21302,8 +21239,8 @@
         <f>SystemicTreatmentI4RC!D11</f>
         <v>Number of cycles/ administrations (O)</v>
       </c>
-      <c r="E12" s="60" t="s">
-        <v>1206</v>
+      <c r="E12" s="3" t="s">
+        <v>1216</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="24" t="s">
@@ -21503,14 +21440,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12E22AA-E82A-4575-B56A-44D33559CD2C}">
   <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21556,7 +21492,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/AdverseEvent</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>AdverseEventI4RC!A2</f>
@@ -21581,7 +21517,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/AdverseEvent</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="C3" s="2" t="str">
         <f>AdverseEventI4RC!A3</f>
@@ -21606,7 +21542,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/AdverseEvent</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="C4" s="2" t="str">
         <f>AdverseEventI4RC!A4</f>
@@ -21631,7 +21567,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/AdverseEvent</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="C5" s="2" t="str">
         <f>AdverseEventI4RC!A5</f>
@@ -21641,15 +21577,15 @@
         <f>AdverseEventI4RC!D5</f>
         <v>Adverse event duration (M)</v>
       </c>
-      <c r="E5" s="35" t="s">
-        <v>1146</v>
+      <c r="E5" s="8" t="s">
+        <v>1209</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
         <v>118</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -21659,17 +21595,19 @@
       <c r="D7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H13" s="36"/>
+      <c r="H13" s="35"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://hl7.eu/fhir/eps/StructureDefinition/Alerts" xr:uid="{F0765931-8736-4740-8DB6-DF1295AE6A41}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{BEBA1B77-9D4F-45AC-BE80-371313DC8EF3}"/>
     <hyperlink ref="A3:A5" r:id="rId3" display="http://hl7.eu/fhir/eps/StructureDefinition/Alerts" xr:uid="{52459153-6409-49E7-A9F6-06FCA66B8F0D}"/>
-    <hyperlink ref="B3:B5" r:id="rId4" display="http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/adverseEvent-eu-i4rc" xr:uid="{EF2863A9-26D6-40BA-A2B8-6B018A7648ED}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{C781A928-F285-404C-B249-093180E7974F}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{B505E530-BAB7-497E-ABC2-48520923F2CA}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{32231032-4E9B-4A60-B38D-04FBD7D69CFA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -21681,7 +21619,6 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21788,7 +21725,6 @@
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3:G4"/>
     </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21959,7 +21895,6 @@
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A13" sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView topLeftCell="D1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21972,7 +21907,7 @@
     <col min="8" max="8" width="54.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>90</v>
       </c>
@@ -21997,7 +21932,7 @@
       <c r="H1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="61"/>
+      <c r="I1" s="59"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22033,7 +21968,7 @@
       <c r="B3" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="61" t="s">
         <v>171</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -23150,11 +23085,8 @@
   </sheetPr>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="B27" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
-    </sheetView>
-    <sheetView topLeftCell="C1" workbookViewId="1">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H30" sqref="B30:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23251,7 +23183,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C4" s="2" t="str">
         <f>ClinicalStageI4RC!A4</f>
@@ -23262,14 +23194,14 @@
         <v>Imaging for primary site (M)</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -23278,7 +23210,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C5" s="2" t="str">
         <f>ClinicalStageI4RC!A5</f>
@@ -23289,14 +23221,14 @@
         <v>CT for primary site (R)</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -23305,7 +23237,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C6" s="2" t="str">
         <f>ClinicalStageI4RC!A6</f>
@@ -23316,14 +23248,14 @@
         <v>MRI for primary site (R)</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -23332,7 +23264,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C7" s="2" t="str">
         <f>ClinicalStageI4RC!A7</f>
@@ -23343,14 +23275,14 @@
         <v>US for primary site (R)</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -23359,7 +23291,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C8" s="2" t="str">
         <f>ClinicalStageI4RC!A8</f>
@@ -23370,14 +23302,14 @@
         <v>Other imaging for primary site (R)</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -23386,7 +23318,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C9" s="2" t="str">
         <f>ClinicalStageI4RC!A9</f>
@@ -23397,14 +23329,14 @@
         <v>Imaging for neck (M)</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -23413,7 +23345,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C10" s="2" t="str">
         <f>ClinicalStageI4RC!A10</f>
@@ -23424,14 +23356,14 @@
         <v>CT for neck (R)</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -23440,7 +23372,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C11" s="2" t="str">
         <f>ClinicalStageI4RC!A11</f>
@@ -23451,14 +23383,14 @@
         <v>MRI for neck (R)</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -23467,7 +23399,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C12" s="2" t="str">
         <f>ClinicalStageI4RC!A12</f>
@@ -23478,14 +23410,14 @@
         <v>US for neck (R)</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -23494,7 +23426,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C13" s="2" t="str">
         <f>ClinicalStageI4RC!A13</f>
@@ -23505,14 +23437,14 @@
         <v>Other imaging for neck (R)</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -23521,7 +23453,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C14" s="2" t="str">
         <f>ClinicalStageI4RC!A14</f>
@@ -23532,14 +23464,14 @@
         <v>Imaging for metastasis (M)</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -23548,7 +23480,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C15" s="2" t="str">
         <f>ClinicalStageI4RC!A15</f>
@@ -23559,14 +23491,14 @@
         <v>CT for metastasis (R)</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -23575,7 +23507,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C16" s="2" t="str">
         <f>ClinicalStageI4RC!A16</f>
@@ -23586,14 +23518,14 @@
         <v>MRI for metastasis (R)</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -23602,7 +23534,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C17" s="2" t="str">
         <f>ClinicalStageI4RC!A17</f>
@@ -23613,14 +23545,14 @@
         <v>US for metastasis (R)</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -23629,7 +23561,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C18" s="2" t="str">
         <f>ClinicalStageI4RC!A18</f>
@@ -23640,14 +23572,14 @@
         <v>Other imaging for metastasis (R)</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -23942,7 +23874,7 @@
         <v>118</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -23969,7 +23901,7 @@
         <v>118</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -23978,7 +23910,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="C31" s="2" t="str">
         <f>ClinicalStageI4RC!A25</f>
@@ -24003,7 +23935,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="C32" s="2" t="str">
         <f>ClinicalStageI4RC!A26</f>
@@ -24017,11 +23949,11 @@
         <v>1087</v>
       </c>
       <c r="F32" s="14"/>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -24030,7 +23962,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="C33" s="2" t="str">
         <f>ClinicalStageI4RC!A27</f>
@@ -24044,11 +23976,11 @@
         <v>1087</v>
       </c>
       <c r="F33" s="14"/>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -24057,7 +23989,7 @@
         <v>http://hl7.eu/fhir/ig/idea4rc/StructureDefinition/ClinicalStage</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="C34" s="2" t="str">
         <f>ClinicalStageI4RC!A28</f>
@@ -24071,11 +24003,11 @@
         <v>1087</v>
       </c>
       <c r="F34" s="14"/>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -24422,10 +24354,9 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>